<commit_message>
more ngrams, asta lemmas, asta form
</commit_message>
<xml_diff>
--- a/methods/ASTA Index Current.xlsx
+++ b/methods/ASTA Index Current.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jodijk\Dropbox\jodijk\Utrecht\Projects\CLARIAH CORE\WP3\VKL\ASTA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jodijk\Dropbox\jodijk\myprograms\python\sastadev\sastadev\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F15E51-326B-4C64-AA03-0ABD5E432C3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE4A462-8887-4F30-A58F-70E2AE576B8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="181">
   <si>
     <t>ID</t>
   </si>
@@ -504,9 +503,6 @@
     <t>post</t>
   </si>
   <si>
-    <t>getlemmas</t>
-  </si>
-  <si>
     <t>A047</t>
   </si>
   <si>
@@ -553,6 +549,36 @@
   </si>
   <si>
     <t>allok</t>
+  </si>
+  <si>
+    <t>substitutie lidwoord</t>
+  </si>
+  <si>
+    <t>del lidwoord</t>
+  </si>
+  <si>
+    <t>delobj</t>
+  </si>
+  <si>
+    <t>delsubj;delsub</t>
+  </si>
+  <si>
+    <t>A049</t>
+  </si>
+  <si>
+    <t>getnounlemmas</t>
+  </si>
+  <si>
+    <t>noun en verb lemmas split up</t>
+  </si>
+  <si>
+    <t>nounlemma</t>
+  </si>
+  <si>
+    <t>verblemma</t>
+  </si>
+  <si>
+    <t>getlexlemmas</t>
   </si>
 </sst>
 </file>
@@ -932,13 +958,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:S48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
+      <selection pane="bottomRight" activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1024,7 +1050,7 @@
         <v>140</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L2" t="s">
         <v>15</v>
@@ -1079,7 +1105,7 @@
         <v>12</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L4" t="s">
         <v>15</v>
@@ -1226,7 +1252,7 @@
         <v>15</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L10" t="s">
         <v>15</v>
@@ -1333,7 +1359,7 @@
         <v>133</v>
       </c>
       <c r="P14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q14" t="s">
         <v>38</v>
@@ -1448,7 +1474,7 @@
         <v>9</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>15</v>
@@ -1458,7 +1484,7 @@
         <v>133</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q19" t="s">
         <v>21</v>
@@ -1487,7 +1513,7 @@
         <v>133</v>
       </c>
       <c r="P20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
@@ -1507,7 +1533,7 @@
         <v>8</v>
       </c>
       <c r="K21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L21" t="s">
         <v>15</v>
@@ -1516,7 +1542,7 @@
         <v>133</v>
       </c>
       <c r="P21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q21" t="s">
         <v>137</v>
@@ -1548,7 +1574,7 @@
         <v>133</v>
       </c>
       <c r="P22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
@@ -1689,7 +1715,7 @@
         <v>15</v>
       </c>
       <c r="N28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
@@ -1782,7 +1808,7 @@
         <v>133</v>
       </c>
       <c r="Q32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
@@ -1795,6 +1821,9 @@
       <c r="E33" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="F33" t="s">
+        <v>171</v>
+      </c>
       <c r="H33" t="s">
         <v>15</v>
       </c>
@@ -1818,6 +1847,9 @@
       <c r="E34" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="F34" t="s">
+        <v>172</v>
+      </c>
       <c r="H34" t="s">
         <v>15</v>
       </c>
@@ -1841,6 +1873,9 @@
       <c r="E35" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="F35" t="s">
+        <v>174</v>
+      </c>
       <c r="H35" t="s">
         <v>15</v>
       </c>
@@ -1933,6 +1968,9 @@
       <c r="E39" s="4" t="s">
         <v>101</v>
       </c>
+      <c r="F39" t="s">
+        <v>173</v>
+      </c>
       <c r="H39" t="s">
         <v>15</v>
       </c>
@@ -2064,7 +2102,7 @@
         <v>15</v>
       </c>
       <c r="N44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
@@ -2074,12 +2112,14 @@
       <c r="D45" t="s">
         <v>153</v>
       </c>
-      <c r="E45" s="4"/>
+      <c r="E45" s="4" t="s">
+        <v>178</v>
+      </c>
       <c r="H45" t="s">
         <v>15</v>
       </c>
       <c r="K45" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="L45" t="s">
         <v>15</v>
@@ -2087,39 +2127,42 @@
       <c r="N45" t="s">
         <v>154</v>
       </c>
+      <c r="Q45" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>155</v>
+      </c>
+      <c r="D46" t="s">
         <v>156</v>
       </c>
-      <c r="D46" t="s">
+      <c r="H46" t="s">
+        <v>15</v>
+      </c>
+      <c r="K46" t="s">
         <v>157</v>
       </c>
-      <c r="H46" t="s">
-        <v>15</v>
-      </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
+        <v>15</v>
+      </c>
+      <c r="N46" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q46" t="s">
         <v>158</v>
-      </c>
-      <c r="L46" t="s">
-        <v>15</v>
-      </c>
-      <c r="N46" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D47" t="s">
         <v>18</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H47" t="s">
         <v>123</v>
@@ -2131,7 +2174,33 @@
         <v>133</v>
       </c>
       <c r="Q47" t="s">
-        <v>164</v>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>175</v>
+      </c>
+      <c r="D48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K48" t="s">
+        <v>180</v>
+      </c>
+      <c r="L48" t="s">
+        <v>15</v>
+      </c>
+      <c r="N48" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ondb changes and more
</commit_message>
<xml_diff>
--- a/methods/ASTA Index Current.xlsx
+++ b/methods/ASTA Index Current.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jodijk\Dropbox\jodijk\myprograms\python\sastadev\sastadev\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE4A462-8887-4F30-A58F-70E2AE576B8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8C3485-58D6-4D69-8677-38623A276157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="185">
   <si>
     <t>ID</t>
   </si>
@@ -579,6 +579,18 @@
   </si>
   <si>
     <t>getlexlemmas</t>
+  </si>
+  <si>
+    <t>delvnw</t>
+  </si>
+  <si>
+    <t>A050</t>
+  </si>
+  <si>
+    <t>pvgetalfout</t>
+  </si>
+  <si>
+    <t>morfpv, congrupv</t>
   </si>
 </sst>
 </file>
@@ -958,13 +970,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S48"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K48" sqref="K48"/>
+      <selection pane="bottomRight" activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1398,6 +1410,9 @@
       <c r="E16" t="s">
         <v>113</v>
       </c>
+      <c r="F16" t="s">
+        <v>181</v>
+      </c>
       <c r="H16" t="s">
         <v>15</v>
       </c>
@@ -2201,6 +2216,32 @@
       </c>
       <c r="Q48" t="s">
         <v>177</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>182</v>
+      </c>
+      <c r="D49" t="s">
+        <v>89</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F49" t="s">
+        <v>184</v>
+      </c>
+      <c r="H49" t="s">
+        <v>123</v>
+      </c>
+      <c r="L49" t="s">
+        <v>15</v>
+      </c>
+      <c r="N49" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
increased typing and doc strings
</commit_message>
<xml_diff>
--- a/methods/ASTA Index Current.xlsx
+++ b/methods/ASTA Index Current.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jodijk\Dropbox\jodijk\myprograms\python\sastadev\sastadev\methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jodijk\Dropbox\jodijk\myprograms\python\sastacode\sastadev\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8C3485-58D6-4D69-8677-38623A276157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D04D538-D843-4C63-B366-C1CFA70BD81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="187">
   <si>
     <t>ID</t>
   </si>
@@ -591,6 +591,12 @@
   </si>
   <si>
     <t>morfpv, congrupv</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -973,10 +979,10 @@
   <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q49" sqref="Q49"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1137,6 +1143,9 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F5" t="s">
         <v>103</v>
       </c>
       <c r="H5" t="s">
@@ -1160,6 +1169,9 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F6" t="s">
         <v>104</v>
       </c>
       <c r="H6" t="s">

</xml_diff>

<commit_message>
ASTA sempar, phonpar, neologisme; documentation
</commit_message>
<xml_diff>
--- a/methods/ASTA Index Current.xlsx
+++ b/methods/ASTA Index Current.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jodijk\Dropbox\jodijk\myprograms\python\sastacode\sastadev\methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Odijk101\Dropbox\jodijk\myprograms\python\sastacode\sastadev\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D04D538-D843-4C63-B366-C1CFA70BD81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF59A08-3A5D-4211-AF65-5901BEF6E07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="190">
   <si>
     <t>ID</t>
   </si>
@@ -597,6 +597,15 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>phonpar</t>
+  </si>
+  <si>
+    <t>sempar</t>
+  </si>
+  <si>
+    <t>neologisme</t>
   </si>
 </sst>
 </file>
@@ -979,10 +988,10 @@
   <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1252,6 +1261,9 @@
       <c r="H9" t="s">
         <v>15</v>
       </c>
+      <c r="K9" t="s">
+        <v>187</v>
+      </c>
       <c r="L9" t="s">
         <v>15</v>
       </c>
@@ -1594,6 +1606,9 @@
       <c r="I22">
         <v>10</v>
       </c>
+      <c r="K22" t="s">
+        <v>189</v>
+      </c>
       <c r="L22" t="s">
         <v>15</v>
       </c>
@@ -1668,6 +1683,9 @@
       </c>
       <c r="H25" t="s">
         <v>15</v>
+      </c>
+      <c r="K25" t="s">
+        <v>188</v>
       </c>
       <c r="L25" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Change QA to Grammaticale fout in ASTA method definition
</commit_message>
<xml_diff>
--- a/methods/ASTA Index Current.xlsx
+++ b/methods/ASTA Index Current.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Odijk101\Dropbox\jodijk\myprograms\python\sastacode\sastadev\methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a3248526/git/sasta/backend/sastadev/methods/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF59A08-3A5D-4211-AF65-5901BEF6E07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68F57BD-A2D6-7A45-B204-09B8A26BBB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$49</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -305,9 +305,6 @@
     <t>A039</t>
   </si>
   <si>
-    <t>QA</t>
-  </si>
-  <si>
     <t>SUBVZ</t>
   </si>
   <si>
@@ -606,6 +603,9 @@
   </si>
   <si>
     <t>neologisme</t>
+  </si>
+  <si>
+    <t>Grammaticale fout</t>
   </si>
 </sst>
 </file>
@@ -988,21 +988,21 @@
   <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K23" sqref="K23"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.109375" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1037,19 +1037,19 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>11</v>
@@ -1057,7 +1057,7 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1068,28 +1068,28 @@
         <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H2" t="s">
         <v>15</v>
       </c>
       <c r="I2" t="s">
+        <v>139</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q2" t="s">
         <v>140</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1109,10 +1109,10 @@
         <v>15</v>
       </c>
       <c r="N3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1132,19 +1132,19 @@
         <v>12</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L4" t="s">
         <v>15</v>
       </c>
       <c r="N4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1152,10 +1152,10 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -1167,10 +1167,10 @@
         <v>15</v>
       </c>
       <c r="N5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1178,10 +1178,10 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -1193,22 +1193,22 @@
         <v>15</v>
       </c>
       <c r="N6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="E7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" t="s">
         <v>107</v>
       </c>
-      <c r="F7" t="s">
-        <v>108</v>
-      </c>
       <c r="H7" t="s">
         <v>15</v>
       </c>
@@ -1216,13 +1216,13 @@
         <v>15</v>
       </c>
       <c r="N7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1242,10 +1242,10 @@
         <v>15</v>
       </c>
       <c r="N8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1256,48 +1256,48 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
       </c>
       <c r="K9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L9" t="s">
         <v>15</v>
       </c>
       <c r="N9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="E10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" t="s">
         <v>120</v>
       </c>
-      <c r="F10" t="s">
-        <v>121</v>
-      </c>
       <c r="H10" t="s">
         <v>15</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L10" t="s">
         <v>15</v>
       </c>
       <c r="N10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1317,10 +1317,10 @@
         <v>15</v>
       </c>
       <c r="N11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1340,10 +1340,10 @@
         <v>15</v>
       </c>
       <c r="N12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1363,10 +1363,10 @@
         <v>15</v>
       </c>
       <c r="N13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -1386,22 +1386,22 @@
         <v>37</v>
       </c>
       <c r="K14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L14" t="s">
         <v>15</v>
       </c>
       <c r="N14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1409,10 +1409,10 @@
         <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
@@ -1421,21 +1421,21 @@
         <v>15</v>
       </c>
       <c r="N15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="E16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
@@ -1444,21 +1444,21 @@
         <v>15</v>
       </c>
       <c r="N16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="E17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
@@ -1467,22 +1467,22 @@
         <v>15</v>
       </c>
       <c r="N17" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="E18" t="s">
+        <v>108</v>
+      </c>
+      <c r="F18" t="s">
         <v>109</v>
       </c>
-      <c r="F18" t="s">
-        <v>110</v>
-      </c>
       <c r="H18" t="s">
         <v>15</v>
       </c>
@@ -1490,13 +1490,13 @@
         <v>15</v>
       </c>
       <c r="N18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -1513,23 +1513,23 @@
         <v>9</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="M19" s="3"/>
       <c r="N19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1543,19 +1543,19 @@
         <v>15</v>
       </c>
       <c r="K20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L20" t="s">
         <v>15</v>
       </c>
       <c r="N20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P20" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1572,22 +1572,22 @@
         <v>8</v>
       </c>
       <c r="K21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L21" t="s">
         <v>15</v>
       </c>
       <c r="N21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q21" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -1595,10 +1595,10 @@
         <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H22" t="s">
         <v>15</v>
@@ -1607,19 +1607,19 @@
         <v>10</v>
       </c>
       <c r="K22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L22" t="s">
         <v>15</v>
       </c>
       <c r="N22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P22" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -1642,10 +1642,10 @@
         <v>15</v>
       </c>
       <c r="N23" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -1659,16 +1659,16 @@
         <v>37</v>
       </c>
       <c r="L24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q24" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -1679,22 +1679,22 @@
         <v>26</v>
       </c>
       <c r="F25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H25" t="s">
         <v>15</v>
       </c>
       <c r="K25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L25" t="s">
         <v>15</v>
       </c>
       <c r="N25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -1708,16 +1708,16 @@
         <v>37</v>
       </c>
       <c r="L26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -1737,10 +1737,10 @@
         <v>15</v>
       </c>
       <c r="N27" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -1754,25 +1754,25 @@
         <v>15</v>
       </c>
       <c r="K28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L28" t="s">
         <v>15</v>
       </c>
       <c r="N28" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>68</v>
       </c>
       <c r="D29" t="s">
+        <v>189</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="H29" t="s">
         <v>15</v>
       </c>
@@ -1780,21 +1780,21 @@
         <v>15</v>
       </c>
       <c r="N29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q29" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>80</v>
       </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H30" t="s">
         <v>15</v>
@@ -1803,21 +1803,21 @@
         <v>15</v>
       </c>
       <c r="N30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>81</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H31" t="s">
         <v>15</v>
@@ -1826,48 +1826,48 @@
         <v>15</v>
       </c>
       <c r="N31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>82</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H32" t="s">
         <v>15</v>
       </c>
       <c r="K32" s="3"/>
       <c r="L32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q32" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>83</v>
       </c>
       <c r="D33" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H33" t="s">
         <v>15</v>
@@ -1876,24 +1876,24 @@
         <v>15</v>
       </c>
       <c r="N33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q33" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>84</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H34" t="s">
         <v>15</v>
@@ -1902,24 +1902,24 @@
         <v>15</v>
       </c>
       <c r="N34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q34" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>85</v>
       </c>
       <c r="D35" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F35" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H35" t="s">
         <v>15</v>
@@ -1928,21 +1928,21 @@
         <v>15</v>
       </c>
       <c r="N35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q35" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>86</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H36" t="s">
         <v>15</v>
@@ -1951,21 +1951,21 @@
         <v>15</v>
       </c>
       <c r="N36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q36" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>87</v>
       </c>
       <c r="D37" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H37" t="s">
         <v>15</v>
@@ -1974,21 +1974,21 @@
         <v>15</v>
       </c>
       <c r="N37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q37" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>88</v>
       </c>
       <c r="D38" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H38" t="s">
         <v>15</v>
@@ -1997,139 +1997,139 @@
         <v>15</v>
       </c>
       <c r="N38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q38" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" t="s">
+        <v>189</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D39" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" s="4" t="s">
+      <c r="F39" t="s">
+        <v>172</v>
+      </c>
+      <c r="H39" t="s">
+        <v>15</v>
+      </c>
+      <c r="L39" t="s">
+        <v>15</v>
+      </c>
+      <c r="N39" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q39" t="s">
         <v>101</v>
       </c>
-      <c r="F39" t="s">
-        <v>173</v>
-      </c>
-      <c r="H39" t="s">
-        <v>15</v>
-      </c>
-      <c r="L39" t="s">
-        <v>15</v>
-      </c>
-      <c r="N39" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" t="s">
+        <v>189</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F40" t="s">
+        <v>147</v>
+      </c>
+      <c r="H40" t="s">
+        <v>122</v>
+      </c>
+      <c r="L40" t="s">
+        <v>15</v>
+      </c>
+      <c r="N40" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>105</v>
       </c>
-      <c r="D40" t="s">
-        <v>89</v>
-      </c>
-      <c r="E40" s="4" t="s">
+      <c r="D41" t="s">
+        <v>189</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H41" t="s">
         <v>122</v>
       </c>
-      <c r="F40" t="s">
+      <c r="L41" t="s">
+        <v>15</v>
+      </c>
+      <c r="N41" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>126</v>
+      </c>
+      <c r="D42" t="s">
+        <v>189</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H42" t="s">
+        <v>122</v>
+      </c>
+      <c r="L42" t="s">
+        <v>15</v>
+      </c>
+      <c r="N42" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>130</v>
+      </c>
+      <c r="D43" t="s">
+        <v>189</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F43" t="s">
         <v>148</v>
       </c>
-      <c r="H40" t="s">
-        <v>123</v>
-      </c>
-      <c r="L40" t="s">
-        <v>15</v>
-      </c>
-      <c r="N40" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>106</v>
-      </c>
-      <c r="D41" t="s">
-        <v>89</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="H41" t="s">
-        <v>123</v>
-      </c>
-      <c r="L41" t="s">
-        <v>15</v>
-      </c>
-      <c r="N41" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>127</v>
-      </c>
-      <c r="D42" t="s">
-        <v>89</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="H42" t="s">
-        <v>123</v>
-      </c>
-      <c r="L42" t="s">
-        <v>15</v>
-      </c>
-      <c r="N42" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q42" t="s">
+      <c r="H43" t="s">
+        <v>122</v>
+      </c>
+      <c r="L43" t="s">
+        <v>15</v>
+      </c>
+      <c r="N43" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q43" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>131</v>
-      </c>
-      <c r="D43" t="s">
-        <v>89</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="F43" t="s">
-        <v>149</v>
-      </c>
-      <c r="H43" t="s">
-        <v>123</v>
-      </c>
-      <c r="L43" t="s">
-        <v>15</v>
-      </c>
-      <c r="N43" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D44" t="s">
         <v>16</v>
@@ -2141,141 +2141,141 @@
         <v>15</v>
       </c>
       <c r="K44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L44" t="s">
         <v>15</v>
       </c>
       <c r="N44" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>151</v>
+      </c>
+      <c r="D45" t="s">
+        <v>152</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="H45" t="s">
+        <v>15</v>
+      </c>
+      <c r="K45" t="s">
+        <v>175</v>
+      </c>
+      <c r="L45" t="s">
+        <v>15</v>
+      </c>
+      <c r="N45" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>154</v>
+      </c>
+      <c r="D46" t="s">
+        <v>155</v>
+      </c>
+      <c r="H46" t="s">
+        <v>15</v>
+      </c>
+      <c r="K46" t="s">
+        <v>156</v>
+      </c>
+      <c r="L46" t="s">
+        <v>15</v>
+      </c>
+      <c r="N46" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>152</v>
-      </c>
-      <c r="D45" t="s">
-        <v>153</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="H45" t="s">
-        <v>15</v>
-      </c>
-      <c r="K45" t="s">
-        <v>176</v>
-      </c>
-      <c r="L45" t="s">
-        <v>15</v>
-      </c>
-      <c r="N45" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>155</v>
-      </c>
-      <c r="D46" t="s">
-        <v>156</v>
-      </c>
-      <c r="H46" t="s">
-        <v>15</v>
-      </c>
-      <c r="K46" t="s">
+      <c r="Q46" t="s">
         <v>157</v>
       </c>
-      <c r="L46" t="s">
-        <v>15</v>
-      </c>
-      <c r="N46" t="s">
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>160</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>161</v>
       </c>
       <c r="D47" t="s">
         <v>18</v>
       </c>
       <c r="E47" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H47" t="s">
+        <v>122</v>
+      </c>
+      <c r="L47" t="s">
+        <v>122</v>
+      </c>
+      <c r="N47" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q47" t="s">
         <v>162</v>
       </c>
-      <c r="H47" t="s">
-        <v>123</v>
-      </c>
-      <c r="L47" t="s">
-        <v>123</v>
-      </c>
-      <c r="N47" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D48" t="s">
+        <v>152</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="H48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K48" t="s">
+        <v>179</v>
+      </c>
+      <c r="L48" t="s">
+        <v>15</v>
+      </c>
+      <c r="N48" t="s">
         <v>153</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="H48" t="s">
-        <v>15</v>
-      </c>
-      <c r="K48" t="s">
-        <v>180</v>
-      </c>
-      <c r="L48" t="s">
-        <v>15</v>
-      </c>
-      <c r="N48" t="s">
-        <v>154</v>
-      </c>
       <c r="Q48" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>181</v>
+      </c>
+      <c r="D49" t="s">
+        <v>189</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D49" t="s">
-        <v>89</v>
-      </c>
-      <c r="E49" s="4" t="s">
+      <c r="F49" t="s">
         <v>183</v>
       </c>
-      <c r="F49" t="s">
-        <v>184</v>
-      </c>
       <c r="H49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L49" t="s">
         <v>15</v>
       </c>
       <c r="N49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S47" xr:uid="{356449EB-3FBE-4443-8528-03CDC854A576}"/>
+  <autoFilter ref="A1:S49" xr:uid="{356449EB-3FBE-4443-8528-03CDC854A576}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N28">
     <sortCondition ref="E2:E28"/>
   </sortState>

</xml_diff>

<commit_message>
Extensions to the method definitions
</commit_message>
<xml_diff>
--- a/methods/ASTA Index Current.xlsx
+++ b/methods/ASTA Index Current.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Odijk101\Dropbox\jodijk\myprograms\python\sastacode\sastadev\methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF59A08-3A5D-4211-AF65-5901BEF6E07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6855CD8-16D2-490C-A156-822BC8850E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$V$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="195">
   <si>
     <t>ID</t>
   </si>
@@ -440,12 +440,6 @@
     <t>CORE</t>
   </si>
   <si>
-    <t>special1</t>
-  </si>
-  <si>
-    <t>special2</t>
-  </si>
-  <si>
     <t>A045</t>
   </si>
   <si>
@@ -606,6 +600,27 @@
   </si>
   <si>
     <t>neologisme</t>
+  </si>
+  <si>
+    <t>stars</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>variants</t>
+  </si>
+  <si>
+    <t>unused1</t>
+  </si>
+  <si>
+    <t>unused2</t>
+  </si>
+  <si>
+    <t>asta_2019</t>
+  </si>
+  <si>
+    <t>asta_future</t>
   </si>
 </sst>
 </file>
@@ -985,13 +1000,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S49"/>
+  <dimension ref="A1:V49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K23" sqref="K23"/>
+      <selection pane="bottomRight" activeCell="Q48" sqref="Q48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,7 +1017,7 @@
     <col min="11" max="11" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1046,18 +1061,27 @@
         <v>132</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>134</v>
+        <v>188</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>135</v>
+        <v>189</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1074,10 +1098,10 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L2" t="s">
         <v>15</v>
@@ -1086,10 +1110,13 @@
         <v>133</v>
       </c>
       <c r="Q2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+      <c r="T2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1112,7 +1139,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1132,7 +1159,7 @@
         <v>12</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L4" t="s">
         <v>15</v>
@@ -1140,11 +1167,11 @@
       <c r="N4" t="s">
         <v>133</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="T4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1152,7 +1179,7 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F5" t="s">
         <v>103</v>
@@ -1170,7 +1197,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1178,7 +1205,7 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F6" t="s">
         <v>104</v>
@@ -1196,7 +1223,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1218,11 +1245,11 @@
       <c r="N7" t="s">
         <v>133</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="T7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1245,7 +1272,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1256,13 +1283,13 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
       </c>
       <c r="K9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="L9" t="s">
         <v>15</v>
@@ -1271,7 +1298,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1288,7 +1315,7 @@
         <v>15</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L10" t="s">
         <v>15</v>
@@ -1297,7 +1324,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1320,7 +1347,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1343,7 +1370,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1366,7 +1393,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1377,7 +1404,7 @@
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -1386,7 +1413,7 @@
         <v>37</v>
       </c>
       <c r="K14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L14" t="s">
         <v>15</v>
@@ -1395,13 +1422,13 @@
         <v>133</v>
       </c>
       <c r="P14" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q14" t="s">
+        <v>168</v>
+      </c>
+      <c r="T14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1424,7 +1451,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1435,7 +1462,7 @@
         <v>113</v>
       </c>
       <c r="F16" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
@@ -1447,7 +1474,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1458,7 +1485,7 @@
         <v>111</v>
       </c>
       <c r="F17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
@@ -1470,7 +1497,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1492,11 +1519,11 @@
       <c r="N18" t="s">
         <v>133</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="T18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -1513,7 +1540,7 @@
         <v>9</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>15</v>
@@ -1523,13 +1550,16 @@
         <v>133</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q19" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1543,7 +1573,7 @@
         <v>15</v>
       </c>
       <c r="K20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L20" t="s">
         <v>15</v>
@@ -1552,10 +1582,10 @@
         <v>133</v>
       </c>
       <c r="P20" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1572,7 +1602,7 @@
         <v>8</v>
       </c>
       <c r="K21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L21" t="s">
         <v>15</v>
@@ -1581,13 +1611,13 @@
         <v>133</v>
       </c>
       <c r="P21" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+      <c r="T21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -1607,7 +1637,7 @@
         <v>10</v>
       </c>
       <c r="K22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L22" t="s">
         <v>15</v>
@@ -1616,10 +1646,10 @@
         <v>133</v>
       </c>
       <c r="P22" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -1645,7 +1675,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -1659,16 +1689,16 @@
         <v>37</v>
       </c>
       <c r="L24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N24" t="s">
         <v>133</v>
       </c>
-      <c r="Q24" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T24" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -1679,13 +1709,13 @@
         <v>26</v>
       </c>
       <c r="F25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H25" t="s">
         <v>15</v>
       </c>
       <c r="K25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="L25" t="s">
         <v>15</v>
@@ -1694,7 +1724,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -1708,16 +1738,16 @@
         <v>37</v>
       </c>
       <c r="L26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N26" t="s">
         <v>133</v>
       </c>
-      <c r="Q26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -1740,7 +1770,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -1754,16 +1784,16 @@
         <v>15</v>
       </c>
       <c r="K28" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L28" t="s">
         <v>15</v>
       </c>
       <c r="N28" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -1782,11 +1812,11 @@
       <c r="N29" t="s">
         <v>133</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="T29" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>80</v>
       </c>
@@ -1805,11 +1835,11 @@
       <c r="N30" t="s">
         <v>133</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="T30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>81</v>
       </c>
@@ -1828,11 +1858,11 @@
       <c r="N31" t="s">
         <v>133</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="T31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -1852,11 +1882,11 @@
       <c r="N32" t="s">
         <v>133</v>
       </c>
-      <c r="Q32" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T32" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>83</v>
       </c>
@@ -1867,7 +1897,7 @@
         <v>94</v>
       </c>
       <c r="F33" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H33" t="s">
         <v>15</v>
@@ -1878,11 +1908,11 @@
       <c r="N33" t="s">
         <v>133</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="T33" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>84</v>
       </c>
@@ -1893,7 +1923,7 @@
         <v>95</v>
       </c>
       <c r="F34" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H34" t="s">
         <v>15</v>
@@ -1904,11 +1934,11 @@
       <c r="N34" t="s">
         <v>133</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="T34" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -1919,7 +1949,7 @@
         <v>96</v>
       </c>
       <c r="F35" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H35" t="s">
         <v>15</v>
@@ -1930,11 +1960,11 @@
       <c r="N35" t="s">
         <v>133</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="T35" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -1953,11 +1983,11 @@
       <c r="N36" t="s">
         <v>133</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="T36" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -1976,11 +2006,11 @@
       <c r="N37" t="s">
         <v>133</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="T37" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -1999,11 +2029,11 @@
       <c r="N38" t="s">
         <v>133</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="T38" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -2014,7 +2044,7 @@
         <v>101</v>
       </c>
       <c r="F39" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H39" t="s">
         <v>15</v>
@@ -2025,11 +2055,11 @@
       <c r="N39" t="s">
         <v>133</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="T39" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>105</v>
       </c>
@@ -2040,7 +2070,7 @@
         <v>122</v>
       </c>
       <c r="F40" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H40" t="s">
         <v>123</v>
@@ -2051,11 +2081,11 @@
       <c r="N40" t="s">
         <v>133</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="T40" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -2074,11 +2104,11 @@
       <c r="N41" t="s">
         <v>133</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="T41" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>127</v>
       </c>
@@ -2097,11 +2127,11 @@
       <c r="N42" t="s">
         <v>133</v>
       </c>
-      <c r="Q42" t="s">
+      <c r="T42" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>131</v>
       </c>
@@ -2112,7 +2142,7 @@
         <v>130</v>
       </c>
       <c r="F43" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H43" t="s">
         <v>123</v>
@@ -2123,13 +2153,13 @@
       <c r="N43" t="s">
         <v>133</v>
       </c>
-      <c r="Q43" t="s">
+      <c r="T43" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D44" t="s">
         <v>16</v>
@@ -2141,73 +2171,73 @@
         <v>15</v>
       </c>
       <c r="K44" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L44" t="s">
         <v>15</v>
       </c>
       <c r="N44" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>150</v>
+      </c>
+      <c r="D45" t="s">
+        <v>151</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H45" t="s">
+        <v>15</v>
+      </c>
+      <c r="K45" t="s">
+        <v>174</v>
+      </c>
+      <c r="L45" t="s">
+        <v>15</v>
+      </c>
+      <c r="N45" t="s">
+        <v>152</v>
+      </c>
+      <c r="T45" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" t="s">
+        <v>154</v>
+      </c>
+      <c r="H46" t="s">
+        <v>15</v>
+      </c>
+      <c r="K46" t="s">
+        <v>155</v>
+      </c>
+      <c r="L46" t="s">
+        <v>15</v>
+      </c>
+      <c r="N46" t="s">
+        <v>158</v>
+      </c>
+      <c r="T46" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>152</v>
-      </c>
-      <c r="D45" t="s">
-        <v>153</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="H45" t="s">
-        <v>15</v>
-      </c>
-      <c r="K45" t="s">
-        <v>176</v>
-      </c>
-      <c r="L45" t="s">
-        <v>15</v>
-      </c>
-      <c r="N45" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>155</v>
-      </c>
-      <c r="D46" t="s">
-        <v>156</v>
-      </c>
-      <c r="H46" t="s">
-        <v>15</v>
-      </c>
-      <c r="K46" t="s">
-        <v>157</v>
-      </c>
-      <c r="L46" t="s">
-        <v>15</v>
-      </c>
-      <c r="N46" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>161</v>
       </c>
       <c r="D47" t="s">
         <v>18</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H47" t="s">
         <v>123</v>
@@ -2219,47 +2249,50 @@
         <v>133</v>
       </c>
       <c r="Q47" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+      <c r="T47" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>173</v>
+      </c>
+      <c r="D48" t="s">
+        <v>151</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="H48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K48" t="s">
+        <v>178</v>
+      </c>
+      <c r="L48" t="s">
+        <v>15</v>
+      </c>
+      <c r="N48" t="s">
+        <v>152</v>
+      </c>
+      <c r="T48" t="s">
         <v>175</v>
       </c>
-      <c r="D48" t="s">
-        <v>153</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="H48" t="s">
-        <v>15</v>
-      </c>
-      <c r="K48" t="s">
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>180</v>
-      </c>
-      <c r="L48" t="s">
-        <v>15</v>
-      </c>
-      <c r="N48" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>182</v>
       </c>
       <c r="D49" t="s">
         <v>89</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F49" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H49" t="s">
         <v>123</v>
@@ -2270,12 +2303,12 @@
       <c r="N49" t="s">
         <v>133</v>
       </c>
-      <c r="Q49" t="s">
-        <v>163</v>
+      <c r="T49" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S47" xr:uid="{356449EB-3FBE-4443-8528-03CDC854A576}"/>
+  <autoFilter ref="A1:V47" xr:uid="{356449EB-3FBE-4443-8528-03CDC854A576}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N28">
     <sortCondition ref="E2:E28"/>
   </sortState>

</xml_diff>

<commit_message>
Treatment of literal queries, version 1
</commit_message>
<xml_diff>
--- a/methods/ASTA Index Current.xlsx
+++ b/methods/ASTA Index Current.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6855CD8-16D2-490C-A156-822BC8850E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5702438-4BE8-4DA4-9AA5-AD3B855DDEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$V$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$W$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="201">
   <si>
     <t>ID</t>
   </si>
@@ -621,6 +621,24 @@
   </si>
   <si>
     <t>asta_future</t>
+  </si>
+  <si>
+    <t>A051</t>
+  </si>
+  <si>
+    <t>noun en verb lemmas together</t>
+  </si>
+  <si>
+    <t>astalemmafilter</t>
+  </si>
+  <si>
+    <t>asta_lemma</t>
+  </si>
+  <si>
+    <t>literal</t>
+  </si>
+  <si>
+    <t>astalemmafunction</t>
   </si>
 </sst>
 </file>
@@ -1000,13 +1018,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V49"/>
+  <dimension ref="A1:W50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q48" sqref="Q48"/>
+      <selection pane="bottomRight" activeCell="O51" sqref="O51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1017,7 +1035,7 @@
     <col min="11" max="11" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1061,27 +1079,30 @@
         <v>132</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="1"/>
       <c r="V1" s="1"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W1" s="1"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1109,14 +1130,14 @@
       <c r="N2" t="s">
         <v>133</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>193</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1139,7 +1160,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1167,11 +1188,11 @@
       <c r="N4" t="s">
         <v>133</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1197,7 +1218,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1223,7 +1244,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1245,11 +1266,11 @@
       <c r="N7" t="s">
         <v>133</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1272,7 +1293,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1298,7 +1319,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1324,7 +1345,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1347,7 +1368,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1370,7 +1391,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1393,7 +1414,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1421,14 +1442,14 @@
       <c r="N14" t="s">
         <v>133</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>168</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1451,7 +1472,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1474,7 +1495,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1497,7 +1518,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1519,11 +1540,11 @@
       <c r="N18" t="s">
         <v>133</v>
       </c>
-      <c r="T18" t="s">
+      <c r="U18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -1549,17 +1570,17 @@
       <c r="N19" t="s">
         <v>133</v>
       </c>
-      <c r="P19" s="3" t="s">
+      <c r="Q19" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
-      <c r="T19" t="s">
+      <c r="T19" s="3"/>
+      <c r="U19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1581,11 +1602,11 @@
       <c r="N20" t="s">
         <v>133</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1610,14 +1631,14 @@
       <c r="N21" t="s">
         <v>133</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>168</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -1645,11 +1666,11 @@
       <c r="N22" t="s">
         <v>133</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -1675,7 +1696,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -1694,11 +1715,11 @@
       <c r="N24" t="s">
         <v>133</v>
       </c>
-      <c r="T24" t="s">
+      <c r="U24" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -1724,7 +1745,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -1743,11 +1764,11 @@
       <c r="N26" t="s">
         <v>133</v>
       </c>
-      <c r="T26" t="s">
+      <c r="U26" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -1770,7 +1791,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -1793,7 +1814,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -1812,11 +1833,11 @@
       <c r="N29" t="s">
         <v>133</v>
       </c>
-      <c r="T29" t="s">
+      <c r="U29" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>80</v>
       </c>
@@ -1835,11 +1856,11 @@
       <c r="N30" t="s">
         <v>133</v>
       </c>
-      <c r="T30" t="s">
+      <c r="U30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>81</v>
       </c>
@@ -1858,11 +1879,11 @@
       <c r="N31" t="s">
         <v>133</v>
       </c>
-      <c r="T31" t="s">
+      <c r="U31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -1882,11 +1903,11 @@
       <c r="N32" t="s">
         <v>133</v>
       </c>
-      <c r="T32" t="s">
+      <c r="U32" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>83</v>
       </c>
@@ -1908,11 +1929,11 @@
       <c r="N33" t="s">
         <v>133</v>
       </c>
-      <c r="T33" t="s">
+      <c r="U33" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>84</v>
       </c>
@@ -1934,11 +1955,11 @@
       <c r="N34" t="s">
         <v>133</v>
       </c>
-      <c r="T34" t="s">
+      <c r="U34" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>85</v>
       </c>
@@ -1960,11 +1981,11 @@
       <c r="N35" t="s">
         <v>133</v>
       </c>
-      <c r="T35" t="s">
+      <c r="U35" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -1983,11 +2004,11 @@
       <c r="N36" t="s">
         <v>133</v>
       </c>
-      <c r="T36" t="s">
+      <c r="U36" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -2006,11 +2027,11 @@
       <c r="N37" t="s">
         <v>133</v>
       </c>
-      <c r="T37" t="s">
+      <c r="U37" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -2029,11 +2050,11 @@
       <c r="N38" t="s">
         <v>133</v>
       </c>
-      <c r="T38" t="s">
+      <c r="U38" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -2055,11 +2076,11 @@
       <c r="N39" t="s">
         <v>133</v>
       </c>
-      <c r="T39" t="s">
+      <c r="U39" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>105</v>
       </c>
@@ -2081,11 +2102,11 @@
       <c r="N40" t="s">
         <v>133</v>
       </c>
-      <c r="T40" t="s">
+      <c r="U40" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -2104,11 +2125,11 @@
       <c r="N41" t="s">
         <v>133</v>
       </c>
-      <c r="T41" t="s">
+      <c r="U41" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>127</v>
       </c>
@@ -2127,11 +2148,11 @@
       <c r="N42" t="s">
         <v>133</v>
       </c>
-      <c r="T42" t="s">
+      <c r="U42" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>131</v>
       </c>
@@ -2153,11 +2174,11 @@
       <c r="N43" t="s">
         <v>133</v>
       </c>
-      <c r="T43" t="s">
+      <c r="U43" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>134</v>
       </c>
@@ -2180,12 +2201,12 @@
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>150</v>
       </c>
       <c r="D45" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>176</v>
@@ -2202,11 +2223,11 @@
       <c r="N45" t="s">
         <v>152</v>
       </c>
-      <c r="T45" t="s">
+      <c r="U45" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>153</v>
       </c>
@@ -2225,11 +2246,11 @@
       <c r="N46" t="s">
         <v>158</v>
       </c>
-      <c r="T46" t="s">
+      <c r="U46" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>159</v>
       </c>
@@ -2248,19 +2269,19 @@
       <c r="N47" t="s">
         <v>133</v>
       </c>
-      <c r="Q47" t="s">
+      <c r="R47" t="s">
         <v>194</v>
       </c>
-      <c r="T47" t="s">
+      <c r="U47" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>173</v>
       </c>
       <c r="D48" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>177</v>
@@ -2277,11 +2298,11 @@
       <c r="N48" t="s">
         <v>152</v>
       </c>
-      <c r="T48" t="s">
+      <c r="U48" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>180</v>
       </c>
@@ -2303,12 +2324,44 @@
       <c r="N49" t="s">
         <v>133</v>
       </c>
-      <c r="T49" t="s">
+      <c r="U49" t="s">
         <v>161</v>
       </c>
     </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>195</v>
+      </c>
+      <c r="D50" t="s">
+        <v>151</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H50" t="s">
+        <v>15</v>
+      </c>
+      <c r="K50" t="s">
+        <v>198</v>
+      </c>
+      <c r="L50" t="s">
+        <v>15</v>
+      </c>
+      <c r="N50" t="s">
+        <v>133</v>
+      </c>
+      <c r="O50" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>197</v>
+      </c>
+      <c r="U50" t="s">
+        <v>196</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:V47" xr:uid="{356449EB-3FBE-4443-8528-03CDC854A576}"/>
+  <autoFilter ref="A1:W47" xr:uid="{356449EB-3FBE-4443-8528-03CDC854A576}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N28">
     <sortCondition ref="E2:E28"/>
   </sortState>

</xml_diff>